<commit_message>
Update 28 Mai 2025
</commit_message>
<xml_diff>
--- a/genre/Genre par Commune.xlsx
+++ b/genre/Genre par Commune.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Procasef_BETPLUS\Application\DashBoard\Dashnoard\genre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0B2016-7054-42A6-8CE4-E46764C5206A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74712C30-D5D6-493B-AFC7-F51DF2D3766C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="11170" xr2:uid="{08D4EB13-FA54-4D57-8161-78CBFCB2003A}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{08D4EB13-FA54-4D57-8161-78CBFCB2003A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>communeSenegal</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>BEMBOU</t>
+  </si>
+  <si>
+    <t>MOUDERY</t>
+  </si>
+  <si>
+    <t>DINDEFELO</t>
   </si>
 </sst>
 </file>
@@ -445,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6103C832-B577-4003-A893-AB784F8D96B8}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -488,18 +494,16 @@
         <v>450</v>
       </c>
       <c r="C2">
-        <v>5054</v>
+        <v>5060</v>
       </c>
       <c r="D2">
-        <v>5504</v>
+        <v>5510</v>
       </c>
       <c r="E2" s="2">
-        <f>(B2*100)/D2</f>
-        <v>8.1758720930232567</v>
+        <v>8.1669691470054442</v>
       </c>
       <c r="F2" s="2">
-        <f>(C2*100)/D2</f>
-        <v>91.824127906976742</v>
+        <v>91.833030852994554</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -507,159 +511,199 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C3">
-        <v>2620</v>
+        <v>3815</v>
       </c>
       <c r="D3">
-        <v>2787</v>
+        <v>4015</v>
       </c>
       <c r="E3" s="2">
-        <v>5.9921062073914602</v>
+        <v>4.9813200498132</v>
       </c>
       <c r="F3" s="2">
-        <v>94.007893792608542</v>
+        <v>95.018679950186808</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="C4">
-        <v>1081</v>
+        <v>953</v>
       </c>
       <c r="D4">
-        <v>1178</v>
+        <v>1002</v>
       </c>
       <c r="E4" s="2">
-        <v>8.2342954159592523</v>
+        <v>4.8902195608782426</v>
       </c>
       <c r="F4" s="2">
-        <v>91.765704584040748</v>
+        <v>95.109780439121764</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>1015</v>
+        <v>97</v>
       </c>
       <c r="C5">
-        <v>5076</v>
+        <v>1081</v>
       </c>
       <c r="D5">
-        <v>6091</v>
+        <v>1178</v>
       </c>
       <c r="E5" s="2">
-        <v>16.66393038909867</v>
+        <v>8.2342954159592523</v>
       </c>
       <c r="F5" s="2">
-        <v>83.336069610901333</v>
+        <v>91.765704584040748</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>482</v>
+        <v>1015</v>
       </c>
       <c r="C6">
-        <v>6420</v>
+        <v>5076</v>
       </c>
       <c r="D6">
-        <v>6902</v>
+        <v>6091</v>
       </c>
       <c r="E6" s="2">
-        <v>6.9834830483917703</v>
+        <v>16.66393038909867</v>
       </c>
       <c r="F6" s="2">
-        <v>93.016516951608224</v>
+        <v>83.336069610901333</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>2381</v>
+        <v>484</v>
       </c>
       <c r="C7">
-        <v>5784</v>
+        <v>6427</v>
       </c>
       <c r="D7">
-        <v>8165</v>
+        <v>6911</v>
       </c>
       <c r="E7" s="2">
-        <v>29.161053276178809</v>
+        <v>7.0033280277817962</v>
       </c>
       <c r="F7" s="2">
-        <v>70.838946723821181</v>
+        <v>92.996671972218209</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>1335</v>
+        <v>2381</v>
       </c>
       <c r="C8">
-        <v>3449</v>
+        <v>5784</v>
       </c>
       <c r="D8">
-        <v>4784</v>
+        <v>8165</v>
       </c>
       <c r="E8" s="2">
-        <v>27.90551839464883</v>
+        <v>29.161053276178809</v>
       </c>
       <c r="F8" s="2">
-        <v>72.094481605351163</v>
+        <v>70.838946723821181</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>1344</v>
+        <v>363</v>
       </c>
       <c r="C9">
-        <v>3041</v>
+        <v>1167</v>
       </c>
       <c r="D9">
-        <v>4385</v>
+        <v>1530</v>
       </c>
       <c r="E9" s="2">
-        <v>30.649942987457241</v>
+        <v>23.725490196078429</v>
       </c>
       <c r="F9" s="2">
-        <v>69.350057012542749</v>
+        <v>76.274509803921561</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>1353</v>
+      </c>
+      <c r="C10">
+        <v>3504</v>
+      </c>
+      <c r="D10">
+        <v>4857</v>
+      </c>
+      <c r="E10" s="2">
+        <v>27.856701667696111</v>
+      </c>
+      <c r="F10" s="2">
+        <v>72.1432983323039</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>1344</v>
+      </c>
+      <c r="C11">
+        <v>3041</v>
+      </c>
+      <c r="D11">
+        <v>4385</v>
+      </c>
+      <c r="E11" s="2">
+        <v>30.649942987457241</v>
+      </c>
+      <c r="F11" s="2">
+        <v>69.350057012542749</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
-        <v>439</v>
-      </c>
-      <c r="C10">
-        <v>1297</v>
-      </c>
-      <c r="D10">
-        <v>1736</v>
-      </c>
-      <c r="E10" s="2">
-        <v>25.288018433179719</v>
-      </c>
-      <c r="F10" s="2">
-        <v>74.71198156682027</v>
+      <c r="B12">
+        <v>800</v>
+      </c>
+      <c r="C12">
+        <v>2650</v>
+      </c>
+      <c r="D12">
+        <v>3450</v>
+      </c>
+      <c r="E12" s="2">
+        <v>23.188405797101449</v>
+      </c>
+      <c r="F12" s="2">
+        <v>76.811594202898547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>